<commit_message>
Couple more things for housekeeping
 On branch main
 Your branch is up to date with 'origin/main'.

 Changes to be committed:
	modified:   EsoCoolingDevice_BlairHolemanVersion/Data from 11.18.21/eso.xlsx
	modified:   EsoCoolingDevice_BlairHolemanVersion/Data from 11.18.21/eso_1.xlsx
	modified:   EsoCoolingDevice_BlairHolemanVersion/Data from 11.18.21/eso_10.xlsx
	modified:   EsoCoolingDevice_BlairHolemanVersion/Data from 11.18.21/eso_11.xlsx
	modified:   EsoCoolingDevice_BlairHolemanVersion/Data from 11.18.21/eso_12.xlsx
</commit_message>
<xml_diff>
--- a/EsoCoolingDevice_BlairHolemanVersion/Data from 11.18.21/eso.xlsx
+++ b/EsoCoolingDevice_BlairHolemanVersion/Data from 11.18.21/eso.xlsx
@@ -6472,8 +6472,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004456E6F65F02304A9EFDC2289E2E3833" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="99f380d18f3f307f6411cd7d315e286c">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="446029cd-d925-4579-bf5d-30ef27c8be74" xmlns:ns3="a883631d-14a9-4c29-9489-4cf8dfc7ddfa" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0b51c68ca466ebae82acd68775f0ee2e" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004456E6F65F02304A9EFDC2289E2E3833" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3a73e0c20dabbbd26d37a7e5134f46d4">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="446029cd-d925-4579-bf5d-30ef27c8be74" xmlns:ns3="a883631d-14a9-4c29-9489-4cf8dfc7ddfa" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="43e0b06db5273548e7a02a88e1971b89" ns2:_="" ns3:_="">
     <xsd:import namespace="446029cd-d925-4579-bf5d-30ef27c8be74"/>
     <xsd:import namespace="a883631d-14a9-4c29-9489-4cf8dfc7ddfa"/>
     <xsd:element name="properties">
@@ -6496,6 +6496,7 @@
                 <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
                 <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
                 <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -6566,6 +6567,11 @@
           <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
         </xsd:sequence>
       </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="23" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="a883631d-14a9-4c29-9489-4cf8dfc7ddfa" elementFormDefault="qualified">
@@ -6729,7 +6735,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB972D87-2D25-4695-8DAE-B9F44BDE2BBC}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{175FB49F-271F-49CF-A1A0-F223AC641EBC}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>